<commit_message>
Iso output changed to ceramic caps
</commit_message>
<xml_diff>
--- a/src/switched/iso/LCSC_Exported_20210303_051402.xlsx
+++ b/src/switched/iso/LCSC_Exported_20210303_051402.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
   <si>
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
@@ -107,24 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">lcsc.com/product-detail/Zener-Diodes_Shandong-Jingdao-Microelectronics-MM1Z30B_C382832.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C487393</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VKME1651J331MV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ymin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD,10x16.5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">330uF ±20% 63V SMD,10x16.5mm Aluminum Electrolytic Capacitors - SMD RoHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lcsc.com/product-detail/Aluminum-Electrolytic-Capacitors-SMD_Ymin-VKME1651J331MV_C487393.html</t>
   </si>
   <si>
     <t xml:space="preserve">C696860</t>
@@ -527,10 +509,10 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -695,56 +677,22 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0.1728</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>1.73</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>17</v>
@@ -762,24 +710,24 @@
         <v>0.36</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>17</v>
@@ -797,25 +745,25 @@
         <v>2.02</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>17</v>
@@ -833,24 +781,24 @@
         <v>3.6</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>17</v>
@@ -868,24 +816,24 @@
         <v>3.04</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>17</v>
@@ -903,24 +851,24 @@
         <v>5.34</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>17</v>
@@ -938,24 +886,24 @@
         <v>0.76</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>17</v>
@@ -973,24 +921,24 @@
         <v>0.46</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>17</v>
@@ -1008,24 +956,24 @@
         <v>1.3</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>17</v>
@@ -1043,26 +991,26 @@
         <v>0.88</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>2512</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>17</v>
@@ -1080,24 +1028,24 @@
         <v>0.51</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>17</v>
@@ -1115,24 +1063,24 @@
         <v>0.41</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>17</v>
@@ -1150,24 +1098,24 @@
         <v>0.26</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>17</v>
@@ -1185,24 +1133,24 @@
         <v>0.31</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>17</v>
@@ -1220,24 +1168,24 @@
         <v>0.54</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>17</v>
@@ -1255,24 +1203,24 @@
         <v>0.36</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>17</v>
@@ -1290,24 +1238,24 @@
         <v>0.4</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>17</v>
@@ -1325,24 +1273,24 @@
         <v>0.54</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>17</v>
@@ -1360,7 +1308,7 @@
         <v>0.55</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>